<commit_message>
Realice las responsabilidades del modelo de dominio enriquesido residentes, tunos y agendas,ademas de cambios en nombre en el event storming
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Event Storming/Reservas - Event Storming.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Event Storming/Reservas - Event Storming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Event Storming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5A7276-D22B-4430-BA65-F4E8B899CC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED61747-3231-454F-81DD-A1D76CD01256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -393,7 +393,7 @@
     <t>Reser-Pol0005</t>
   </si>
   <si>
-    <t>No es posible tener una reserva con un turno para el mismo residente.</t>
+    <t>No es posible tener dos reserva con un mismo turno para el mismo residente.</t>
   </si>
 </sst>
 </file>
@@ -905,6 +905,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -929,16 +950,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -947,12 +980,15 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -965,9 +1001,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -992,7 +1025,26 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1001,65 +1053,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1182,7 +1182,7 @@
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
+      <sheetData sheetId="2" refreshError="1">
         <row r="11">
           <cell r="D11" t="str">
             <v>Contexto cuya motivación es encargarce de manejar la información de los residentes, incluidas sus identificaciones, contacto, y la relación entre el residente y su residencia dentro del conjunto.</v>
@@ -1566,7 +1566,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4:D6"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1582,22 +1582,22 @@
       <c r="A1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="35" t="str">
+      <c r="B2" s="42" t="str">
         <f>[1]Contextos!$D$14</f>
         <v>Contexto cuya intención enfocarse en la gestión del proceso de reservas de los recursos, incluyendo la disponibilidad de los recursos y las reservas que los residentes realizan.</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
@@ -1623,7 +1623,7 @@
       <c r="C4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="37" t="str">
+      <c r="D4" s="44" t="str">
         <f>$B$1</f>
         <v>Reservas</v>
       </c>
@@ -1638,7 +1638,7 @@
       <c r="C5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="45"/>
     </row>
     <row r="6" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
@@ -1650,7 +1650,7 @@
       <c r="C6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1673,7 +1673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10:H12"/>
     </sheetView>
@@ -1702,84 +1702,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="49" t="str">
+      <c r="B2" s="61" t="str">
         <f>'[2]Listado Objetos Dominio'!A6</f>
         <v>Turno</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="62"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="51" t="str">
+      <c r="B3" s="63" t="str">
         <f>'[2]Listado Objetos Dominio'!B6</f>
         <v>Objeto de dominio que representa uno de los turnos que representan un bloque de tiempo que el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55" t="s">
+      <c r="F4" s="65"/>
+      <c r="G4" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="55"/>
+      <c r="H4" s="66"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1789,52 +1789,52 @@
       <c r="K4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="68" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="58" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="60" t="s">
+      <c r="H5" s="69"/>
+      <c r="I5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="J5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="46"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="12" t="s">
         <v>21</v>
       </c>
@@ -1847,43 +1847,43 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
     </row>
     <row r="7" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48" t="s">
+      <c r="I7" s="55"/>
+      <c r="J7" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48" t="s">
+      <c r="K7" s="55"/>
+      <c r="L7" s="55" t="s">
         <v>35</v>
       </c>
       <c r="M7" s="27" t="s">
@@ -1891,103 +1891,103 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48" t="s">
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="55"/>
     </row>
     <row r="10" spans="1:14" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48" t="s">
+      <c r="I10" s="55"/>
+      <c r="J10" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="48" t="s">
+      <c r="K10" s="47"/>
+      <c r="L10" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="48" t="s">
+      <c r="M10" s="55" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
+      <c r="A12" s="55"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
     </row>
     <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
@@ -2027,36 +2027,36 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="40" t="s">
+      <c r="H14" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="43" t="s">
+      <c r="I14" s="47"/>
+      <c r="J14" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40" t="s">
+      <c r="K14" s="47"/>
+      <c r="L14" s="47" t="s">
         <v>34</v>
       </c>
       <c r="M14" s="31" t="s">
@@ -2064,19 +2064,19 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="80" t="s">
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="36" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2097,22 +2097,28 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
@@ -2129,29 +2135,23 @@
     <mergeCell ref="H7:H9"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="I7:I9"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="L7:L9"/>
     <mergeCell ref="J7:J9"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{18720746-9CC1-4260-8E4D-17DD35D9F7E5}"/>
@@ -2215,63 +2215,63 @@
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="49" t="str">
+      <c r="B2" s="61" t="str">
         <f>'Listado Objetos de Dominio'!A6</f>
         <v>Residente</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="62"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="51" t="str">
+      <c r="B3" s="63" t="str">
         <f>'Listado Objetos de Dominio'!B6</f>
         <v>Objeto de dominio que representa a un residente que vive dentro de un inmueble en un conjunto residencial</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55" t="s">
+      <c r="F4" s="65"/>
+      <c r="G4" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="55"/>
+      <c r="H4" s="66"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2281,52 +2281,52 @@
       <c r="K4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="68" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="58" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="60" t="s">
+      <c r="H5" s="69"/>
+      <c r="I5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="J5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="46"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="12" t="s">
         <v>21</v>
       </c>
@@ -2339,86 +2339,86 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="43" t="str">
+      <c r="B7" s="49" t="str">
         <f>_xlfn.CONCAT("Registrar ",B2)</f>
         <v>Registrar Residente</v>
       </c>
-      <c r="C7" s="43" t="str">
+      <c r="C7" s="49" t="str">
         <f>_xlfn.CONCAT("Acción de registrar un ",B2," para un conjunto residencial.")</f>
         <v>Acción de registrar un Residente para un conjunto residencial.</v>
       </c>
-      <c r="D7" s="43" t="str">
+      <c r="D7" s="49" t="str">
         <f>B2</f>
         <v>Residente</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43" t="str">
+      <c r="I7" s="49"/>
+      <c r="J7" s="49" t="str">
         <f>_xlfn.CONCAT(B2," registrado")</f>
         <v>Residente registrado</v>
       </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43" t="str">
+      <c r="K7" s="49"/>
+      <c r="L7" s="49" t="str">
         <f>_xlfn.CONCAT(B2," eliminado")</f>
         <v>Residente eliminado</v>
       </c>
-      <c r="M7" s="71" t="s">
+      <c r="M7" s="33" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="72"/>
+      <c r="A8" s="77"/>
       <c r="B8" s="73"/>
       <c r="C8" s="73"/>
       <c r="D8" s="73"/>
       <c r="E8" s="73"/>
       <c r="F8" s="73"/>
       <c r="G8" s="73"/>
-      <c r="H8" s="48"/>
+      <c r="H8" s="55"/>
       <c r="I8" s="73"/>
       <c r="J8" s="73"/>
       <c r="K8" s="73"/>
       <c r="L8" s="73"/>
-      <c r="M8" s="71" t="str">
+      <c r="M8" s="33" t="str">
         <f>_xlfn.CONCAT("Buscar ",B2)</f>
         <v>Buscar Residente</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="71" t="str">
+      <c r="A9" s="78"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="33" t="str">
         <f>_xlfn.CONCAT("Eliminar ",B2)</f>
         <v>Eliminar Residente</v>
       </c>
@@ -2457,71 +2457,71 @@
         <v>Residente modificado</v>
       </c>
       <c r="K10" s="27"/>
-      <c r="L10" s="40" t="str">
+      <c r="L10" s="47" t="str">
         <f>_xlfn.CONCAT(B2," registrado")</f>
         <v>Residente registrado</v>
       </c>
-      <c r="M10" s="71" t="str">
+      <c r="M10" s="33" t="str">
         <f>_xlfn.CONCAT("Eliminar ",$B$2)</f>
         <v>Eliminar Residente</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="43" t="str">
+      <c r="B11" s="49" t="str">
         <f>_xlfn.CONCAT("Buscar ",B2)</f>
         <v>Buscar Residente</v>
       </c>
-      <c r="C11" s="43" t="str">
+      <c r="C11" s="49" t="str">
         <f>_xlfn.CONCAT("Acción de buscar la información asociada a un ",B2," del conjunto residencial.")</f>
         <v>Acción de buscar la información asociada a un Residente del conjunto residencial.</v>
       </c>
-      <c r="D11" s="43" t="str">
+      <c r="D11" s="49" t="str">
         <f>B2</f>
         <v>Residente</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="49" t="s">
         <v>81</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43" t="str">
+      <c r="I11" s="49"/>
+      <c r="J11" s="49" t="str">
         <f>_xlfn.CONCAT(B2," buscado")</f>
         <v>Residente buscado</v>
       </c>
-      <c r="K11" s="43"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="71" t="str">
+      <c r="K11" s="49"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="33" t="str">
         <f>_xlfn.CONCAT("Modificar ",$B$2)</f>
         <v>Modificar Residente</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="76"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
+      <c r="A12" s="75"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="77" t="str">
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="34" t="str">
         <f>_xlfn.CONCAT("Eliminar ",$B$2)</f>
         <v>Eliminar Residente</v>
       </c>
@@ -2560,17 +2560,41 @@
         <v>Residente eliminado</v>
       </c>
       <c r="K13" s="27"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="71" t="str">
+      <c r="L13" s="48"/>
+      <c r="M13" s="33" t="str">
         <f>_xlfn.CONCAT("Crear ",$B$2)</f>
         <v>Crear Residente</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E14" s="78"/>
+      <c r="E14" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="L10:L13"/>
@@ -2587,30 +2611,6 @@
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{827E654C-67F5-45D4-9416-536CC2969F91}"/>
@@ -2624,8 +2624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8893E27C-63FD-4248-8D03-DE2849BD7525}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M11"/>
+    <sheetView topLeftCell="A4" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2652,84 +2652,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="49" t="str">
+      <c r="B2" s="61" t="str">
         <f>'Listado Objetos de Dominio'!A4</f>
         <v>Reserva</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="62"/>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="51" t="str">
+      <c r="B3" s="63" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada una de las reservas creadas por los residente según una zona comun que esta condicionada con una agenda y según la disponibilidad de turno poder reservar el espacio.</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55" t="s">
+      <c r="F4" s="65"/>
+      <c r="G4" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="55"/>
+      <c r="H4" s="66"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2739,52 +2739,52 @@
       <c r="K4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="68" t="s">
+      <c r="L4" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="69" t="s">
+      <c r="M4" s="85" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="58" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="60" t="s">
+      <c r="H5" s="69"/>
+      <c r="I5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="61" t="s">
+      <c r="J5" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="68"/>
-      <c r="M5" s="69"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="85"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="46"/>
+      <c r="A6" s="58"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="12" t="s">
         <v>21</v>
       </c>
@@ -2797,29 +2797,29 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="69"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="84"/>
+      <c r="M6" s="85"/>
     </row>
     <row r="7" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="47" t="s">
         <v>57</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -2829,24 +2829,24 @@
         <v>75</v>
       </c>
       <c r="I7" s="11"/>
-      <c r="J7" s="65" t="s">
+      <c r="J7" s="51" t="s">
         <v>98</v>
       </c>
       <c r="K7" s="11"/>
-      <c r="L7" s="65" t="s">
+      <c r="L7" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="85" t="s">
+      <c r="M7" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="82"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="41"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="54"/>
       <c r="G8" s="11" t="s">
         <v>61</v>
       </c>
@@ -2854,20 +2854,20 @@
         <v>62</v>
       </c>
       <c r="I8" s="11"/>
-      <c r="J8" s="66"/>
+      <c r="J8" s="52"/>
       <c r="K8" s="11"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="85" t="s">
+      <c r="L8" s="52"/>
+      <c r="M8" s="39" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="82"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="41"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="11" t="s">
         <v>63</v>
       </c>
@@ -2875,20 +2875,20 @@
         <v>64</v>
       </c>
       <c r="I9" s="11"/>
-      <c r="J9" s="66"/>
+      <c r="J9" s="52"/>
       <c r="K9" s="11"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="65" t="s">
+      <c r="L9" s="52"/>
+      <c r="M9" s="51" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="82"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="41"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="25" t="s">
         <v>101</v>
       </c>
@@ -2896,18 +2896,18 @@
         <v>60</v>
       </c>
       <c r="I10" s="25"/>
-      <c r="J10" s="66"/>
+      <c r="J10" s="52"/>
       <c r="K10" s="25"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
     </row>
     <row r="11" spans="1:14" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="64"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="42"/>
+      <c r="A11" s="82"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="25" t="s">
         <v>102</v>
       </c>
@@ -2915,43 +2915,43 @@
         <v>103</v>
       </c>
       <c r="I11" s="25"/>
-      <c r="J11" s="67"/>
+      <c r="J11" s="53"/>
       <c r="K11" s="25"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="67"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
     </row>
     <row r="12" spans="1:14" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="65" t="s">
+      <c r="D12" s="52"/>
+      <c r="E12" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="40" t="s">
+      <c r="G12" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I12" s="65"/>
-      <c r="J12" s="81" t="s">
+      <c r="I12" s="51"/>
+      <c r="J12" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="65"/>
-      <c r="L12" s="81" t="s">
+      <c r="K12" s="51"/>
+      <c r="L12" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="M12" s="84" t="s">
+      <c r="M12" s="37" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2959,18 +2959,18 @@
       <c r="A13" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="84" t="s">
+      <c r="B13" s="53"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="80"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="37" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2978,89 +2978,89 @@
       <c r="A14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65" t="s">
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="K14" s="65"/>
-      <c r="L14" s="65" t="s">
+      <c r="K14" s="51"/>
+      <c r="L14" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="M14" s="84" t="s">
+      <c r="M14" s="37" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="66"/>
-      <c r="M15" s="84" t="s">
+      <c r="B15" s="54"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="37" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="64"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="84" t="s">
+      <c r="A16" s="82"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="37" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="83" t="s">
+      <c r="A17" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65" t="s">
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65" t="s">
+      <c r="K17" s="51"/>
+      <c r="L17" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="M17" s="81" t="s">
+      <c r="M17" s="80" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3068,21 +3068,55 @@
       <c r="A18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="81"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="G12:G18"/>
+    <mergeCell ref="H12:H18"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="D7:D18"/>
+    <mergeCell ref="E12:E18"/>
+    <mergeCell ref="F12:F18"/>
     <mergeCell ref="M9:M11"/>
     <mergeCell ref="M17:M18"/>
     <mergeCell ref="A15:A16"/>
@@ -3099,40 +3133,6 @@
     <mergeCell ref="L17:L18"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="D7:D18"/>
-    <mergeCell ref="E12:E18"/>
-    <mergeCell ref="F12:F18"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="G12:G18"/>
-    <mergeCell ref="H12:H18"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{804E2C57-E5A8-4901-8BC4-4B63A7C4FA3E}"/>
@@ -3145,21 +3145,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C279D002CEC08F42B7087C30E58D0266" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5713f579c7011938dc4987ae8981b8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3219184d-29ab-4105-b29c-8e343e335d59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae0a0ff84a3c6712467f60982d6e378d" ns2:_="">
     <xsd:import namespace="3219184d-29ab-4105-b29c-8e343e335d59"/>
@@ -3303,10 +3288,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3219184d-29ab-4105-b29c-8e343e335d59"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3329,19 +3339,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3219184d-29ab-4105-b29c-8e343e335d59"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>